<commit_message>
try overflow for mobile
</commit_message>
<xml_diff>
--- a/data/mcdonalds_prices_new.xlsx
+++ b/data/mcdonalds_prices_new.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Github/would_you_like_some_fries_with_that/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A2AD9D-4A1A-974E-BFA0-F22E57B252C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516062F9-3343-5342-B6DC-FB39C3588E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$641</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -646,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D641"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A500" workbookViewId="0">
+      <selection activeCell="C509" sqref="C509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1981,7 +1984,7 @@
         <v>2.4500000000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>35</v>
       </c>
@@ -1991,8 +1994,11 @@
       <c r="C97" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D97">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>35</v>
       </c>
@@ -2002,8 +2008,11 @@
       <c r="C98" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D98">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>35</v>
       </c>
@@ -2013,8 +2022,11 @@
       <c r="C99" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D99">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>35</v>
       </c>
@@ -2024,8 +2036,11 @@
       <c r="C100" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D100">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>35</v>
       </c>
@@ -2035,8 +2050,11 @@
       <c r="C101" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D101">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>35</v>
       </c>
@@ -2046,8 +2064,11 @@
       <c r="C102" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D102">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>35</v>
       </c>
@@ -2057,8 +2078,11 @@
       <c r="C103" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D103">
+        <v>5.95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>35</v>
       </c>
@@ -2068,8 +2092,11 @@
       <c r="C104" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D104">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>35</v>
       </c>
@@ -2079,8 +2106,11 @@
       <c r="C105" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D105">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>35</v>
       </c>
@@ -2090,8 +2120,11 @@
       <c r="C106" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D106">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>35</v>
       </c>
@@ -2101,8 +2134,11 @@
       <c r="C107" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D107">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>35</v>
       </c>
@@ -2112,8 +2148,11 @@
       <c r="C108" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D108">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>35</v>
       </c>
@@ -2123,8 +2162,11 @@
       <c r="C109" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D109">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>35</v>
       </c>
@@ -2134,8 +2176,11 @@
       <c r="C110" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>35</v>
       </c>
@@ -2145,8 +2190,11 @@
       <c r="C111" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D111">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>35</v>
       </c>
@@ -2155,6 +2203,9 @@
       </c>
       <c r="C112" t="s">
         <v>6</v>
+      </c>
+      <c r="D112">
+        <v>7.1</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2167,6 +2218,9 @@
       <c r="C113" t="s">
         <v>6</v>
       </c>
+      <c r="D113">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
@@ -9080,7 +9134,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="609" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
         <v>35</v>
       </c>
@@ -9090,8 +9144,11 @@
       <c r="C609" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="610" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D609">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
         <v>35</v>
       </c>
@@ -9101,8 +9158,11 @@
       <c r="C610" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="611" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D610">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
         <v>35</v>
       </c>
@@ -9112,8 +9172,11 @@
       <c r="C611" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="612" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D611">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
         <v>35</v>
       </c>
@@ -9123,8 +9186,11 @@
       <c r="C612" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="613" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D612">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>35</v>
       </c>
@@ -9134,8 +9200,11 @@
       <c r="C613" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="614" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D613">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
         <v>35</v>
       </c>
@@ -9145,8 +9214,11 @@
       <c r="C614" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="615" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D614">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
         <v>35</v>
       </c>
@@ -9156,8 +9228,11 @@
       <c r="C615" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="616" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D615">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>35</v>
       </c>
@@ -9167,8 +9242,11 @@
       <c r="C616" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="617" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D616">
+        <v>6.85</v>
+      </c>
+    </row>
+    <row r="617" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
         <v>35</v>
       </c>
@@ -9178,8 +9256,11 @@
       <c r="C617" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="618" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D617">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
         <v>35</v>
       </c>
@@ -9189,8 +9270,11 @@
       <c r="C618" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="619" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D618">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="619" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A619" t="s">
         <v>35</v>
       </c>
@@ -9200,8 +9284,11 @@
       <c r="C619" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="620" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D619">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="620" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A620" t="s">
         <v>35</v>
       </c>
@@ -9211,8 +9298,11 @@
       <c r="C620" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="621" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D620">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A621" t="s">
         <v>35</v>
       </c>
@@ -9222,8 +9312,11 @@
       <c r="C621" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="622" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D621">
+        <v>6.55</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
         <v>35</v>
       </c>
@@ -9233,8 +9326,11 @@
       <c r="C622" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="623" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D622">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
         <v>35</v>
       </c>
@@ -9244,8 +9340,11 @@
       <c r="C623" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="624" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D623">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
         <v>35</v>
       </c>
@@ -9254,6 +9353,9 @@
       </c>
       <c r="C624" t="s">
         <v>51</v>
+      </c>
+      <c r="D624">
+        <v>8.3000000000000007</v>
       </c>
     </row>
     <row r="625" spans="1:4" x14ac:dyDescent="0.2">
@@ -9266,6 +9368,9 @@
       <c r="C625" t="s">
         <v>51</v>
       </c>
+      <c r="D625">
+        <v>6.75</v>
+      </c>
     </row>
     <row r="626" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
@@ -9492,6 +9597,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D641" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update mcd.ipynb prep for distance analysis
</commit_message>
<xml_diff>
--- a/data/mcdonalds_prices_new.xlsx
+++ b/data/mcdonalds_prices_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Github/would_you_like_some_fries_with_that/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC0FC97-F89C-214C-87C8-3E73B44E91BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D9779E-51E0-AA4B-9216-1E38D05E8022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -890,7 +890,7 @@
   <dimension ref="A1:E641"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>